<commit_message>
Refactoring of Solitaire domain classes. Removed unnecessary test.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02617424-EC07-4057-BEAE-DCEF89B7FCC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FD9999-0B4E-4D25-9D5E-3831CCDAEC62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -192,6 +192,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>265802</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>132832</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E6D66B-5CBE-4B54-A50A-E34E536BB606}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2219325" y="0"/>
+          <a:ext cx="7180952" cy="4142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,7 +543,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,5 +691,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated domain logic after call on 22/01/20.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FD9999-0B4E-4D25-9D5E-3831CCDAEC62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A538CC-448A-4703-B51F-7EA473446630}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -199,15 +199,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>265802</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>132832</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>27110</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -230,8 +230,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2219325" y="0"/>
-          <a:ext cx="7180952" cy="4142857"/>
+          <a:off x="1971675" y="0"/>
+          <a:ext cx="6667500" cy="3846635"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -543,7 +543,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added class and set up initial logic for "Foundation". Added unit tests for initialization of foundation.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2679D5B1-FE91-4300-83B8-5D90D42D55D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CD78AA-4E89-4E0F-99D3-F61EC45B2B81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Card</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>FoundationPile (4x)</t>
   </si>
 </sst>
 </file>
@@ -558,15 +561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -667,67 +670,100 @@
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>6</v>
+      <c r="A24" t="s">
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B32" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated excel file. Deleted uneeded test.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2947B5A-B612-4FAA-AE2E-166F50427067}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9BD1C4-2ADA-4E42-9D37-F13C24EF7FC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Card</t>
   </si>
@@ -69,12 +69,6 @@
     <t>StockCards</t>
   </si>
   <si>
-    <t>TableauCards</t>
-  </si>
-  <si>
-    <t>FoundationCards</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -105,7 +99,37 @@
     <t>int</t>
   </si>
   <si>
-    <t>FoundationPile (4x)</t>
+    <t>FoundationPileClubs</t>
+  </si>
+  <si>
+    <t>FoundationPileDiamonds</t>
+  </si>
+  <si>
+    <t>FoundationPileHearts</t>
+  </si>
+  <si>
+    <t>FoundationPileSpades</t>
+  </si>
+  <si>
+    <t>TableauPile1</t>
+  </si>
+  <si>
+    <t>TableauPile2</t>
+  </si>
+  <si>
+    <t>TableauPile3</t>
+  </si>
+  <si>
+    <t>TableauPile4</t>
+  </si>
+  <si>
+    <t>TableauPile5</t>
+  </si>
+  <si>
+    <t>TableauPile6</t>
+  </si>
+  <si>
+    <t>TableauPile7</t>
   </si>
 </sst>
 </file>
@@ -191,13 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,30 +586,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -623,15 +648,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +669,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -652,7 +677,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -660,10 +685,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,91 +698,123 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
+      <c r="A21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>10</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B38" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started creating Tableau logic. Tests are to be added.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9BD1C4-2ADA-4E42-9D37-F13C24EF7FC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EF4D64-041D-4915-BE4E-0D302B463B46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>Card</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>TableauPile7</t>
+  </si>
+  <si>
+    <t>IsOpen</t>
+  </si>
+  <si>
+    <t>IsClosed</t>
   </si>
 </sst>
 </file>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,57 +714,75 @@
       <c r="A20" t="s">
         <v>27</v>
       </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -766,55 +790,71 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>18</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Board logic and tests for moving card from tableau pile to another tableau pile.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EF4D64-041D-4915-BE4E-0D302B463B46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE34D983-F5E8-434E-92B8-1A10F60974D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Card</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>IsClosed</t>
+  </si>
+  <si>
+    <t>Move card from tableau to tableau</t>
+  </si>
+  <si>
+    <t>Move card from waste to tableau</t>
+  </si>
+  <si>
+    <t>Move card to foundation  from tableau or from waste</t>
+  </si>
+  <si>
+    <t>DrawFromStock</t>
+  </si>
+  <si>
+    <t>If card was moved out of tableau pile a new one should be opened</t>
+  </si>
+  <si>
+    <t>Check the win condition</t>
   </si>
 </sst>
 </file>
@@ -592,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
@@ -812,7 +830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -820,21 +838,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -842,7 +878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -850,7 +886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
If target pile is empty and the card to be moved has Rank Kind, it can be moved to anempty pile. Associated unit test has been added.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Solution\Solitaire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE34D983-F5E8-434E-92B8-1A10F60974D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29640031-E393-408D-B0BE-74263D948B4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Card</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Check the win condition</t>
+  </si>
+  <si>
+    <t>Move King from tableau to empty pile</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -247,6 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +853,7 @@
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="7" t="s">
         <v>35</v>
       </c>
       <c r="I36" t="s">
@@ -884,6 +894,9 @@
       </c>
       <c r="B39" t="s">
         <v>7</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added logic for new open card. If card was moved from tableau to tableau the next card becomes open. If card could not be moved open card is still the same.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29640031-E393-408D-B0BE-74263D948B4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54994130-2F6B-44E2-B67D-F238B85D7869}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Board</t>
   </si>
   <si>
-    <t>Waste</t>
-  </si>
-  <si>
     <t>Stock</t>
   </si>
   <si>
@@ -150,13 +147,16 @@
     <t>DrawFromStock</t>
   </si>
   <si>
-    <t>If card was moved out of tableau pile a new one should be opened</t>
-  </si>
-  <si>
     <t>Check the win condition</t>
   </si>
   <si>
     <t>Move King from tableau to empty pile</t>
+  </si>
+  <si>
+    <t>If card was moved out of tableau pile a new one should be opened on the origin pile</t>
+  </si>
+  <si>
+    <t>CardCanBeMoved</t>
   </si>
 </sst>
 </file>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,16 +634,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,20 +682,20 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -719,20 +719,20 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
         <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -788,29 +788,36 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -818,7 +825,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -826,7 +833,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -834,7 +841,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -842,10 +849,10 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
         <v>18</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -854,57 +861,51 @@
         <v>6</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I36" t="s">
-        <v>37</v>
-      </c>
-      <c r="O36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O37" t="s">
         <v>38</v>
-      </c>
-      <c r="O37" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic and tests for moving cards from stock to tableau,
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DA11E7-AB3F-41CC-B4E1-7C976363C2F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0169B8-963F-4B6A-842F-BBCCDE223A03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added board tests for drawing cards from stock.
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0169B8-963F-4B6A-842F-BBCCDE223A03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0347F7D1-D428-4F74-B72E-46FF20B7FA04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBB0860-A6A0-48AC-9068-29105113A1C6}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +874,10 @@
       <c r="B37" t="s">
         <v>8</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="7" t="s">
         <v>37</v>
       </c>
       <c r="O37" t="s">

</xml_diff>

<commit_message>
Code refactoring (access modifiers, removing unneeded methods and properties)
</commit_message>
<xml_diff>
--- a/Solitaire/BackEndApplication.xlsx
+++ b/Solitaire/BackEndApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raman Khosravi\source\repos\Raman2503\Solution\Solitaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0033C1-A5F8-448A-8E51-741F2E423C8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF95795-7060-4F54-80C2-9FE4FBC96A7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B2662D-53B7-4411-A568-85960054B7A3}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>